<commit_message>
bugs, publication ready plots
</commit_message>
<xml_diff>
--- a/analysis/results/Q1/models/supplements_models_colon.xlsx
+++ b/analysis/results/Q1/models/supplements_models_colon.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -89,37 +89,37 @@
     <t xml:space="preserve">pre_ltx vs healthy ASV colon</t>
   </si>
   <si>
-    <t xml:space="preserve">0.986997377622378</t>
+    <t xml:space="preserve">0.927801242236025</t>
   </si>
   <si>
     <t xml:space="preserve">pre_ltx vs post_ltx ASV colon</t>
   </si>
   <si>
-    <t xml:space="preserve">0.925719448990726</t>
+    <t xml:space="preserve">0.925942693409742</t>
   </si>
   <si>
     <t xml:space="preserve">post_ltx vs healthy ASV colon</t>
   </si>
   <si>
-    <t xml:space="preserve">0.976036965398668</t>
+    <t xml:space="preserve">0.970100909430672</t>
   </si>
   <si>
     <t xml:space="preserve">pre_ltx vs healthy genus colon</t>
   </si>
   <si>
-    <t xml:space="preserve">0.940304487179487</t>
+    <t xml:space="preserve">0.942347826086957</t>
   </si>
   <si>
     <t xml:space="preserve">pre_ltx vs post_ltx genus colon</t>
   </si>
   <si>
-    <t xml:space="preserve">0.826906028368794</t>
+    <t xml:space="preserve">0.873348571428571</t>
   </si>
   <si>
     <t xml:space="preserve">post_ltx vs healthy genus colon</t>
   </si>
   <si>
-    <t xml:space="preserve">0.969267139479905</t>
+    <t xml:space="preserve">0.95301685891748</t>
   </si>
   <si>
     <t xml:space="preserve">mtry</t>
@@ -215,7 +215,31 @@
     <t xml:space="preserve">0.991512345679012</t>
   </si>
   <si>
-    <t xml:space="preserve">0.994408074195308</t>
+    <t xml:space="preserve">0.994934097421203</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.997367216117216</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.990964266230224</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.961211428571429</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.983595352016405</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.923076923076923</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.999485359361136</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.999194157642911</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.999785084891468</t>
   </si>
   <si>
     <t xml:space="preserve">0.915557729941292</t>
@@ -236,22 +260,22 @@
     <t xml:space="preserve">0.887432995830852</t>
   </si>
   <si>
-    <t xml:space="preserve">0.957969114219114</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.75216516639389</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.974263915753277</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.959498834498835</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.853024413529733</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.967386632280249</t>
+    <t xml:space="preserve">0.946981366459627</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.885312320916905</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.898805816084999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.956782608695652</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.880657142857143</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.937897071872227</t>
   </si>
 </sst>
 </file>
@@ -812,31 +836,31 @@
         <v>22</v>
       </c>
       <c r="B8" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
         <v>23</v>
       </c>
       <c r="D8" t="n">
-        <v>0.775974993750258</v>
+        <v>0.839062275964413</v>
       </c>
       <c r="E8" t="n">
-        <v>0.678230913026368</v>
+        <v>0.763516514084874</v>
       </c>
       <c r="F8" t="n">
-        <v>0.845617513257423</v>
+        <v>0.903653108076064</v>
       </c>
       <c r="G8" t="n">
-        <v>0.824817518248175</v>
+        <v>0.815085158150852</v>
       </c>
       <c r="H8" t="n">
-        <v>0.759512404209416</v>
+        <v>0.749621505068144</v>
       </c>
       <c r="I8" t="n">
-        <v>0.704245090016367</v>
+        <v>0.686077355011733</v>
       </c>
       <c r="J8" t="n">
-        <v>0.817514822134387</v>
+        <v>0.817763440860215</v>
       </c>
     </row>
     <row r="9">
@@ -850,25 +874,25 @@
         <v>25</v>
       </c>
       <c r="D9" t="n">
-        <v>0.578667827753082</v>
+        <v>0.631284080000009</v>
       </c>
       <c r="E9" t="n">
-        <v>0.534101501867895</v>
+        <v>0.548366604970915</v>
       </c>
       <c r="F9" t="n">
-        <v>0.637071814926527</v>
+        <v>0.718554348300078</v>
       </c>
       <c r="G9" t="n">
-        <v>0.845272206303725</v>
+        <v>0.836393989983305</v>
       </c>
       <c r="H9" t="n">
-        <v>0.566833906226995</v>
+        <v>0.60687703928205</v>
       </c>
       <c r="I9" t="n">
-        <v>0.511591551104263</v>
+        <v>0.512612107623318</v>
       </c>
       <c r="J9" t="n">
-        <v>0.611807568438003</v>
+        <v>0.685306306306306</v>
       </c>
     </row>
     <row r="10">
@@ -882,25 +906,25 @@
         <v>27</v>
       </c>
       <c r="D10" t="n">
-        <v>0.860514028859966</v>
+        <v>0.864752886244012</v>
       </c>
       <c r="E10" t="n">
-        <v>0.757009187894485</v>
+        <v>0.804976965351386</v>
       </c>
       <c r="F10" t="n">
-        <v>0.976605017006803</v>
+        <v>0.901255490667008</v>
       </c>
       <c r="G10" t="n">
-        <v>0.893719806763285</v>
+        <v>0.901960784313726</v>
       </c>
       <c r="H10" t="n">
-        <v>0.793139356150599</v>
+        <v>0.825267950557022</v>
       </c>
       <c r="I10" t="n">
-        <v>0.684217634574571</v>
+        <v>0.806831395348837</v>
       </c>
       <c r="J10" t="n">
-        <v>0.878891257995736</v>
+        <v>0.846629881154499</v>
       </c>
     </row>
     <row r="11">
@@ -908,31 +932,31 @@
         <v>28</v>
       </c>
       <c r="B11" t="n">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
         <v>29</v>
       </c>
       <c r="D11" t="n">
-        <v>0.847486537072107</v>
+        <v>0.860826823814835</v>
       </c>
       <c r="E11" t="n">
-        <v>0.761305694523722</v>
+        <v>0.815622168476863</v>
       </c>
       <c r="F11" t="n">
-        <v>0.887908430818879</v>
+        <v>0.898361004025808</v>
       </c>
       <c r="G11" t="n">
-        <v>0.883211678832117</v>
+        <v>0.851581508515815</v>
       </c>
       <c r="H11" t="n">
-        <v>0.806243548300781</v>
+        <v>0.76383364066034</v>
       </c>
       <c r="I11" t="n">
-        <v>0.709873327484097</v>
+        <v>0.718907399789753</v>
       </c>
       <c r="J11" t="n">
-        <v>0.84626976284585</v>
+        <v>0.80698732718894</v>
       </c>
     </row>
     <row r="12">
@@ -940,31 +964,31 @@
         <v>30</v>
       </c>
       <c r="B12" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
         <v>31</v>
       </c>
       <c r="D12" t="n">
-        <v>0.521115220535476</v>
+        <v>0.653791417350769</v>
       </c>
       <c r="E12" t="n">
-        <v>0.424149693107756</v>
+        <v>0.541840953979724</v>
       </c>
       <c r="F12" t="n">
-        <v>0.60714063161916</v>
+        <v>0.72277552899821</v>
       </c>
       <c r="G12" t="n">
-        <v>0.71919770773639</v>
+        <v>0.78</v>
       </c>
       <c r="H12" t="n">
-        <v>0.527600257585189</v>
+        <v>0.613972148232613</v>
       </c>
       <c r="I12" t="n">
-        <v>0.445538565463031</v>
+        <v>0.517405705996131</v>
       </c>
       <c r="J12" t="n">
-        <v>0.570085817524842</v>
+        <v>0.691212584708856</v>
       </c>
     </row>
     <row r="13">
@@ -972,31 +996,31 @@
         <v>32</v>
       </c>
       <c r="B13" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
         <v>33</v>
       </c>
       <c r="D13" t="n">
-        <v>0.899210232516894</v>
+        <v>0.888220110634547</v>
       </c>
       <c r="E13" t="n">
-        <v>0.824873820656258</v>
+        <v>0.849961010792007</v>
       </c>
       <c r="F13" t="n">
-        <v>0.987783952866861</v>
+        <v>0.919499276501051</v>
       </c>
       <c r="G13" t="n">
-        <v>0.893719806763285</v>
+        <v>0.839530332681018</v>
       </c>
       <c r="H13" t="n">
-        <v>0.816933673353169</v>
+        <v>0.749617644808842</v>
       </c>
       <c r="I13" t="n">
-        <v>0.73546277665996</v>
+        <v>0.679520114298521</v>
       </c>
       <c r="J13" t="n">
-        <v>0.95073929115025</v>
+        <v>0.801953173041446</v>
       </c>
     </row>
   </sheetData>
@@ -1284,7 +1308,7 @@
         <v>22</v>
       </c>
       <c r="B8" t="n">
-        <v>117</v>
+        <v>143</v>
       </c>
       <c r="C8" t="s">
         <v>37</v>
@@ -1296,25 +1320,25 @@
         <v>38</v>
       </c>
       <c r="F8" t="n">
-        <v>0.949794111013738</v>
+        <v>0.959906853066139</v>
       </c>
       <c r="G8" t="n">
-        <v>0.888534638648126</v>
+        <v>0.917894596040663</v>
       </c>
       <c r="H8" t="n">
-        <v>0.989691207601044</v>
+        <v>0.990534751636504</v>
       </c>
       <c r="I8" t="n">
         <v>1</v>
       </c>
       <c r="J8" t="n">
-        <v>0.921224018783099</v>
+        <v>0.898408204093909</v>
       </c>
       <c r="K8" t="n">
-        <v>0.856105169340463</v>
+        <v>0.841650541795666</v>
       </c>
       <c r="L8" t="n">
-        <v>0.971569055944056</v>
+        <v>0.941198156682028</v>
       </c>
     </row>
     <row r="9">
@@ -1322,7 +1346,7 @@
         <v>24</v>
       </c>
       <c r="B9" t="n">
-        <v>99</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
         <v>37</v>
@@ -1334,25 +1358,25 @@
         <v>38</v>
       </c>
       <c r="F9" t="n">
-        <v>0.680815160801924</v>
+        <v>0.794527112030982</v>
       </c>
       <c r="G9" t="n">
-        <v>0.580433785766691</v>
+        <v>0.75868816717499</v>
       </c>
       <c r="H9" t="n">
-        <v>0.747201861422146</v>
+        <v>0.838290901476989</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0.634458980156123</v>
+        <v>0.723064714497306</v>
       </c>
       <c r="K9" t="n">
-        <v>0.585509289980093</v>
+        <v>0.680063699497912</v>
       </c>
       <c r="L9" t="n">
-        <v>0.721376388077148</v>
+        <v>0.779712749615975</v>
       </c>
     </row>
     <row r="10">
@@ -1360,7 +1384,7 @@
         <v>26</v>
       </c>
       <c r="B10" t="n">
-        <v>363</v>
+        <v>237</v>
       </c>
       <c r="C10" t="s">
         <v>37</v>
@@ -1372,25 +1396,25 @@
         <v>38</v>
       </c>
       <c r="F10" t="n">
-        <v>0.869948606149641</v>
+        <v>0.917730699555073</v>
       </c>
       <c r="G10" t="n">
-        <v>0.777975817286162</v>
+        <v>0.878634330461583</v>
       </c>
       <c r="H10" t="n">
-        <v>0.951673347910593</v>
+        <v>0.950989966082533</v>
       </c>
       <c r="I10" t="n">
         <v>1</v>
       </c>
       <c r="J10" t="n">
-        <v>0.823616968362975</v>
+        <v>0.881796676401075</v>
       </c>
       <c r="K10" t="n">
-        <v>0.708466955579632</v>
+        <v>0.837513456937799</v>
       </c>
       <c r="L10" t="n">
-        <v>0.928313253012048</v>
+        <v>0.929279005877843</v>
       </c>
     </row>
     <row r="11">
@@ -1398,7 +1422,7 @@
         <v>28</v>
       </c>
       <c r="B11" t="n">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
         <v>37</v>
@@ -1410,25 +1434,25 @@
         <v>38</v>
       </c>
       <c r="F11" t="n">
-        <v>0.888618290073723</v>
+        <v>0.9548542694099</v>
       </c>
       <c r="G11" t="n">
-        <v>0.761565259544035</v>
+        <v>0.903490025891711</v>
       </c>
       <c r="H11" t="n">
-        <v>0.950002750098218</v>
+        <v>0.990457346263093</v>
       </c>
       <c r="I11" t="n">
         <v>1</v>
       </c>
       <c r="J11" t="n">
-        <v>0.851008059836108</v>
+        <v>0.891176421396033</v>
       </c>
       <c r="K11" t="n">
-        <v>0.748882978723404</v>
+        <v>0.829713166275561</v>
       </c>
       <c r="L11" t="n">
-        <v>0.911580658268996</v>
+        <v>0.936596638655462</v>
       </c>
     </row>
     <row r="12">
@@ -1436,37 +1460,37 @@
         <v>30</v>
       </c>
       <c r="B12" t="n">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="C12" t="s">
         <v>37</v>
       </c>
       <c r="D12" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E12" t="s">
         <v>38</v>
       </c>
       <c r="F12" t="n">
-        <v>0.679340296835686</v>
+        <v>0.786300409895636</v>
       </c>
       <c r="G12" t="n">
-        <v>0.612471867233133</v>
+        <v>0.721433337977152</v>
       </c>
       <c r="H12" t="n">
-        <v>0.759515233468216</v>
+        <v>0.86765150894798</v>
       </c>
       <c r="I12" t="n">
         <v>1</v>
       </c>
       <c r="J12" t="n">
-        <v>0.62692618415362</v>
+        <v>0.698873203516184</v>
       </c>
       <c r="K12" t="n">
-        <v>0.561761750154607</v>
+        <v>0.631400784885591</v>
       </c>
       <c r="L12" t="n">
-        <v>0.682653490328007</v>
+        <v>0.788145456693844</v>
       </c>
     </row>
     <row r="13">
@@ -1474,7 +1498,7 @@
         <v>32</v>
       </c>
       <c r="B13" t="n">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="C13" t="s">
         <v>37</v>
@@ -1486,25 +1510,25 @@
         <v>38</v>
       </c>
       <c r="F13" t="n">
-        <v>0.921860991241497</v>
+        <v>0.932916990774884</v>
       </c>
       <c r="G13" t="n">
-        <v>0.86736385349238</v>
+        <v>0.898368390221042</v>
       </c>
       <c r="H13" t="n">
-        <v>0.962331800852209</v>
+        <v>0.990651837992141</v>
       </c>
       <c r="I13" t="n">
         <v>1</v>
       </c>
       <c r="J13" t="n">
-        <v>0.870248742899904</v>
+        <v>0.88837455040854</v>
       </c>
       <c r="K13" t="n">
-        <v>0.774093043107128</v>
+        <v>0.861981585484394</v>
       </c>
       <c r="L13" t="n">
-        <v>0.929218308327897</v>
+        <v>0.936565751445087</v>
       </c>
     </row>
   </sheetData>
@@ -1813,7 +1837,7 @@
         <v>22</v>
       </c>
       <c r="B8" t="n">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="C8" t="n">
         <v>3</v>
@@ -1822,31 +1846,31 @@
         <v>0.1</v>
       </c>
       <c r="E8" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F8" t="s">
         <v>38</v>
       </c>
       <c r="G8" t="n">
-        <v>0.947817899440924</v>
+        <v>0.971139143531829</v>
       </c>
       <c r="H8" t="n">
-        <v>0.896744157740993</v>
+        <v>0.941090658021712</v>
       </c>
       <c r="I8" t="n">
-        <v>0.989040500813973</v>
+        <v>0.995027081757913</v>
       </c>
       <c r="J8" t="n">
         <v>1</v>
       </c>
       <c r="K8" t="n">
-        <v>0.921003521101515</v>
+        <v>0.921728316771981</v>
       </c>
       <c r="L8" t="n">
-        <v>0.88212443584784</v>
+        <v>0.879595588235294</v>
       </c>
       <c r="M8" t="n">
-        <v>0.952155904842821</v>
+        <v>0.963986013986014</v>
       </c>
     </row>
     <row r="9">
@@ -1863,31 +1887,31 @@
         <v>0.1</v>
       </c>
       <c r="E9" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F9" t="s">
         <v>38</v>
       </c>
       <c r="G9" t="n">
-        <v>0.742156389697318</v>
+        <v>0.806227491018711</v>
       </c>
       <c r="H9" t="n">
-        <v>0.698768594723309</v>
+        <v>0.755988111058377</v>
       </c>
       <c r="I9" t="n">
-        <v>0.81681179848884</v>
+        <v>0.8528396759471</v>
       </c>
       <c r="J9" t="n">
         <v>1</v>
       </c>
       <c r="K9" t="n">
-        <v>0.682869070773598</v>
+        <v>0.73107125788158</v>
       </c>
       <c r="L9" t="n">
-        <v>0.629610125646711</v>
+        <v>0.656692546583851</v>
       </c>
       <c r="M9" t="n">
-        <v>0.717357571214393</v>
+        <v>0.8001996996997</v>
       </c>
     </row>
     <row r="10">
@@ -1898,37 +1922,37 @@
         <v>500</v>
       </c>
       <c r="C10" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D10" t="n">
         <v>0.1</v>
       </c>
       <c r="E10" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F10" t="s">
         <v>38</v>
       </c>
       <c r="G10" t="n">
-        <v>0.936405563583694</v>
+        <v>0.964363091926635</v>
       </c>
       <c r="H10" t="n">
-        <v>0.881963137680554</v>
+        <v>0.940122431671388</v>
       </c>
       <c r="I10" t="n">
-        <v>0.998979591836735</v>
+        <v>0.985828858111928</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>
       </c>
       <c r="K10" t="n">
-        <v>0.894336146970896</v>
+        <v>0.924948985295538</v>
       </c>
       <c r="L10" t="n">
-        <v>0.824630058834017</v>
+        <v>0.893441174807779</v>
       </c>
       <c r="M10" t="n">
-        <v>0.980555555555556</v>
+        <v>0.950549450549451</v>
       </c>
     </row>
     <row r="11">
@@ -1939,37 +1963,37 @@
         <v>500</v>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D11" t="n">
         <v>0.1</v>
       </c>
       <c r="E11" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F11" t="s">
         <v>38</v>
       </c>
       <c r="G11" t="n">
-        <v>0.950571860156772</v>
+        <v>0.968444116177032</v>
       </c>
       <c r="H11" t="n">
-        <v>0.867373015558811</v>
+        <v>0.940941094501065</v>
       </c>
       <c r="I11" t="n">
-        <v>0.989882852959034</v>
+        <v>0.992296098864074</v>
       </c>
       <c r="J11" t="n">
         <v>1</v>
       </c>
       <c r="K11" t="n">
-        <v>0.900681313282912</v>
+        <v>0.907370789649755</v>
       </c>
       <c r="L11" t="n">
-        <v>0.772582205029014</v>
+        <v>0.884882288806332</v>
       </c>
       <c r="M11" t="n">
-        <v>0.945263612352702</v>
+        <v>0.945</v>
       </c>
     </row>
     <row r="12">
@@ -1986,31 +2010,31 @@
         <v>0.1</v>
       </c>
       <c r="E12" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F12" t="s">
         <v>38</v>
       </c>
       <c r="G12" t="n">
-        <v>0.709429736904851</v>
+        <v>0.808901484272791</v>
       </c>
       <c r="H12" t="n">
-        <v>0.65183473023637</v>
+        <v>0.752702256712158</v>
       </c>
       <c r="I12" t="n">
-        <v>0.75506515812694</v>
+        <v>0.88789342144142</v>
       </c>
       <c r="J12" t="n">
         <v>1</v>
       </c>
       <c r="K12" t="n">
-        <v>0.658365885758715</v>
+        <v>0.71848825427861</v>
       </c>
       <c r="L12" t="n">
-        <v>0.578353297840875</v>
+        <v>0.65693208380691</v>
       </c>
       <c r="M12" t="n">
-        <v>0.761662028838857</v>
+        <v>0.800416227608008</v>
       </c>
     </row>
     <row r="13">
@@ -2018,7 +2042,7 @@
         <v>32</v>
       </c>
       <c r="B13" t="n">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="C13" t="n">
         <v>3</v>
@@ -2033,25 +2057,25 @@
         <v>38</v>
       </c>
       <c r="G13" t="n">
-        <v>0.931532632297962</v>
+        <v>0.96566635637558</v>
       </c>
       <c r="H13" t="n">
-        <v>0.869564868908521</v>
+        <v>0.930899856848133</v>
       </c>
       <c r="I13" t="n">
-        <v>0.996938775510204</v>
+        <v>0.991255084933279</v>
       </c>
       <c r="J13" t="n">
         <v>1</v>
       </c>
       <c r="K13" t="n">
-        <v>0.900444648782833</v>
+        <v>0.921415511428119</v>
       </c>
       <c r="L13" t="n">
-        <v>0.784443021766965</v>
+        <v>0.877127659574468</v>
       </c>
       <c r="M13" t="n">
-        <v>0.992857142857143</v>
+        <v>0.95739161849711</v>
       </c>
     </row>
   </sheetData>
@@ -2405,25 +2429,25 @@
         <v>0.4</v>
       </c>
       <c r="C8" t="n">
-        <v>0.00960631053638794</v>
+        <v>0.0014538327873387</v>
       </c>
       <c r="D8" t="s">
         <v>38</v>
       </c>
-      <c r="E8" t="e">
-        <v>#NUM!</v>
+      <c r="E8" t="s">
+        <v>38</v>
       </c>
       <c r="F8" t="s">
         <v>38</v>
       </c>
       <c r="G8" t="n">
-        <v>0.947591655103159</v>
+        <v>0.958045499079975</v>
       </c>
       <c r="H8" t="n">
-        <v>0.899070840323319</v>
+        <v>0.919974493090533</v>
       </c>
       <c r="I8" t="n">
-        <v>0.974258611552729</v>
+        <v>0.979096385542169</v>
       </c>
       <c r="J8" t="n">
         <v>1</v>
@@ -2435,13 +2459,13 @@
         <v>1</v>
       </c>
       <c r="M8" t="n">
-        <v>0.892267727889019</v>
+        <v>0.896262269761579</v>
       </c>
       <c r="N8" t="n">
-        <v>0.862237493128092</v>
+        <v>0.844885708182012</v>
       </c>
       <c r="O8" t="n">
-        <v>0.922722016651249</v>
+        <v>0.933223776223776</v>
       </c>
     </row>
     <row r="9">
@@ -2449,46 +2473,46 @@
         <v>24</v>
       </c>
       <c r="B9" t="n">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0137046689762817</v>
+        <v>0.00859715072274094</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" t="e">
-        <v>#NUM!</v>
+        <v>65</v>
+      </c>
+      <c r="E9" t="s">
+        <v>66</v>
       </c>
       <c r="F9" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="G9" t="n">
-        <v>0.620119931619318</v>
+        <v>0.693086870904058</v>
       </c>
       <c r="H9" t="n">
-        <v>0.463295502819712</v>
+        <v>0.599715148965813</v>
       </c>
       <c r="I9" t="n">
-        <v>0.703052443629767</v>
+        <v>0.758895467736863</v>
       </c>
       <c r="J9" t="n">
-        <v>1</v>
+        <v>0.954924874791319</v>
       </c>
       <c r="K9" t="e">
         <v>#NUM!</v>
       </c>
       <c r="L9" t="n">
-        <v>1</v>
+        <v>0.936962750716332</v>
       </c>
       <c r="M9" t="n">
-        <v>0.611546292413607</v>
+        <v>0.65861441757332</v>
       </c>
       <c r="N9" t="n">
-        <v>0.517056619995087</v>
+        <v>0.578956424254241</v>
       </c>
       <c r="O9" t="n">
-        <v>0.686149425287356</v>
+        <v>0.714558558558559</v>
       </c>
     </row>
     <row r="10">
@@ -2496,28 +2520,28 @@
         <v>26</v>
       </c>
       <c r="B10" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0155848751740653</v>
+        <v>0.0107158795058739</v>
       </c>
       <c r="D10" t="s">
         <v>38</v>
       </c>
-      <c r="E10" t="e">
-        <v>#NUM!</v>
+      <c r="E10" t="s">
+        <v>38</v>
       </c>
       <c r="F10" t="s">
         <v>38</v>
       </c>
       <c r="G10" t="n">
-        <v>0.933330787797685</v>
+        <v>0.927875231047784</v>
       </c>
       <c r="H10" t="n">
-        <v>0.835665149027218</v>
+        <v>0.884389329519448</v>
       </c>
       <c r="I10" t="n">
-        <v>0.99515723490685</v>
+        <v>0.965489372572735</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>
@@ -2529,13 +2553,13 @@
         <v>1</v>
       </c>
       <c r="M10" t="n">
-        <v>0.89119077550448</v>
+        <v>0.868252682268749</v>
       </c>
       <c r="N10" t="n">
-        <v>0.804032413660043</v>
+        <v>0.82293956043956</v>
       </c>
       <c r="O10" t="n">
-        <v>0.96838262139467</v>
+        <v>0.91311500999001</v>
       </c>
     </row>
     <row r="11">
@@ -2543,28 +2567,28 @@
         <v>28</v>
       </c>
       <c r="B11" t="n">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="C11" t="n">
-        <v>0.00801880134902893</v>
+        <v>0.00534451465450061</v>
       </c>
       <c r="D11" t="s">
         <v>38</v>
       </c>
-      <c r="E11" t="e">
-        <v>#NUM!</v>
+      <c r="E11" t="s">
+        <v>38</v>
       </c>
       <c r="F11" t="s">
         <v>38</v>
       </c>
       <c r="G11" t="n">
-        <v>0.93235079693475</v>
+        <v>0.941556387930976</v>
       </c>
       <c r="H11" t="n">
-        <v>0.876282619279455</v>
+        <v>0.911600992222732</v>
       </c>
       <c r="I11" t="n">
-        <v>0.967590092503304</v>
+        <v>0.972603350921737</v>
       </c>
       <c r="J11" t="n">
         <v>1</v>
@@ -2576,13 +2600,13 @@
         <v>1</v>
       </c>
       <c r="M11" t="n">
-        <v>0.867933193933055</v>
+        <v>0.892543469634242</v>
       </c>
       <c r="N11" t="n">
-        <v>0.835989304812834</v>
+        <v>0.856537556639944</v>
       </c>
       <c r="O11" t="n">
-        <v>0.909881422924901</v>
+        <v>0.916957057735772</v>
       </c>
     </row>
     <row r="12">
@@ -2590,46 +2614,46 @@
         <v>30</v>
       </c>
       <c r="B12" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0132969831442191</v>
+        <v>0.0544456176964336</v>
       </c>
       <c r="D12" t="s">
-        <v>65</v>
-      </c>
-      <c r="E12" t="e">
-        <v>#NUM!</v>
+        <v>68</v>
+      </c>
+      <c r="E12" t="s">
+        <v>69</v>
       </c>
       <c r="F12" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="G12" t="n">
-        <v>0.569037250100923</v>
+        <v>0.713578224881508</v>
       </c>
       <c r="H12" t="n">
-        <v>0.491666288101473</v>
+        <v>0.648353848088962</v>
       </c>
       <c r="I12" t="n">
-        <v>0.709651582054504</v>
+        <v>0.788408871575181</v>
       </c>
       <c r="J12" t="n">
-        <v>0.959885386819484</v>
+        <v>0.886666666666667</v>
       </c>
       <c r="K12" t="e">
         <v>#NUM!</v>
       </c>
       <c r="L12" t="n">
-        <v>0.959885386819484</v>
+        <v>0.842406876790831</v>
       </c>
       <c r="M12" t="n">
-        <v>0.575685448354478</v>
+        <v>0.655676030198237</v>
       </c>
       <c r="N12" t="n">
-        <v>0.510444382852919</v>
+        <v>0.617904898499559</v>
       </c>
       <c r="O12" t="n">
-        <v>0.691254503345342</v>
+        <v>0.716055497014401</v>
       </c>
     </row>
     <row r="13">
@@ -2637,46 +2661,46 @@
         <v>32</v>
       </c>
       <c r="B13" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>0.0142332462121855</v>
+        <v>0.0361260232689994</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" t="e">
-        <v>#NUM!</v>
+        <v>71</v>
+      </c>
+      <c r="E13" t="s">
+        <v>72</v>
       </c>
       <c r="F13" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="G13" t="n">
-        <v>0.931308643899931</v>
+        <v>0.907412761343259</v>
       </c>
       <c r="H13" t="n">
-        <v>0.829138321995465</v>
+        <v>0.859075369075369</v>
       </c>
       <c r="I13" t="n">
-        <v>0.999672011661808</v>
+        <v>0.938341688671997</v>
       </c>
       <c r="J13" t="n">
-        <v>1</v>
+        <v>0.986301369863014</v>
       </c>
       <c r="K13" t="e">
         <v>#NUM!</v>
       </c>
       <c r="L13" t="n">
-        <v>1</v>
+        <v>0.990338164251208</v>
       </c>
       <c r="M13" t="n">
-        <v>0.88561761249765</v>
+        <v>0.849756423612702</v>
       </c>
       <c r="N13" t="n">
-        <v>0.775639658848614</v>
+        <v>0.807443169278305</v>
       </c>
       <c r="O13" t="n">
-        <v>0.964481409001957</v>
+        <v>0.893489161849711</v>
       </c>
     </row>
   </sheetData>
@@ -2733,7 +2757,7 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D2" t="n">
         <v>0.828821576743759</v>
@@ -2765,7 +2789,7 @@
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D3" t="n">
         <v>0.665626979544435</v>
@@ -2797,7 +2821,7 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="D4" t="n">
         <v>0.824173140590477</v>
@@ -2829,7 +2853,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="D5" t="n">
         <v>0.818786794265407</v>
@@ -2861,7 +2885,7 @@
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="D6" t="n">
         <v>0.718261925015855</v>
@@ -2893,7 +2917,7 @@
         <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="D7" t="n">
         <v>0.800987555073082</v>
@@ -2922,31 +2946,31 @@
         <v>22</v>
       </c>
       <c r="B8" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="D8" t="n">
-        <v>0.854344652491684</v>
+        <v>0.831386465854944</v>
       </c>
       <c r="E8" t="n">
-        <v>0.723443254506687</v>
+        <v>0.762305868747047</v>
       </c>
       <c r="F8" t="n">
-        <v>0.934751811069255</v>
+        <v>0.912787220309811</v>
       </c>
       <c r="G8" t="n">
-        <v>0.916058394160584</v>
+        <v>0.841849148418491</v>
       </c>
       <c r="H8" t="n">
-        <v>0.823132774804462</v>
+        <v>0.728074183753592</v>
       </c>
       <c r="I8" t="n">
-        <v>0.732005623242737</v>
+        <v>0.606546052631579</v>
       </c>
       <c r="J8" t="n">
-        <v>0.916478615946701</v>
+        <v>0.839592760180995</v>
       </c>
     </row>
     <row r="9">
@@ -2954,31 +2978,31 @@
         <v>24</v>
       </c>
       <c r="B9" t="n">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="D9" t="n">
-        <v>0.54176154822385</v>
+        <v>0.646110164127784</v>
       </c>
       <c r="E9" t="n">
-        <v>0.460468545020871</v>
+        <v>0.557633504887205</v>
       </c>
       <c r="F9" t="n">
-        <v>0.629955035613118</v>
+        <v>0.69594175170068</v>
       </c>
       <c r="G9" t="n">
-        <v>0.713467048710602</v>
+        <v>0.782971619365609</v>
       </c>
       <c r="H9" t="n">
-        <v>0.540623904482125</v>
+        <v>0.599831322555652</v>
       </c>
       <c r="I9" t="n">
-        <v>0.452197697950923</v>
+        <v>0.543546458541676</v>
       </c>
       <c r="J9" t="n">
-        <v>0.60404047976012</v>
+        <v>0.650647342995169</v>
       </c>
     </row>
     <row r="10">
@@ -2986,31 +3010,31 @@
         <v>26</v>
       </c>
       <c r="B10" t="n">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D10" t="n">
-        <v>0.887988189604785</v>
+        <v>0.783304252458454</v>
       </c>
       <c r="E10" t="n">
-        <v>0.841975723140496</v>
+        <v>0.718171542830033</v>
       </c>
       <c r="F10" t="n">
-        <v>0.959870019436346</v>
+        <v>0.834550380579376</v>
       </c>
       <c r="G10" t="n">
-        <v>0.898550724637681</v>
+        <v>0.847058823529412</v>
       </c>
       <c r="H10" t="n">
-        <v>0.793371368353981</v>
+        <v>0.739839497509308</v>
       </c>
       <c r="I10" t="n">
-        <v>0.727087662951067</v>
+        <v>0.694838164931044</v>
       </c>
       <c r="J10" t="n">
-        <v>0.895634920634921</v>
+        <v>0.795947680950088</v>
       </c>
     </row>
     <row r="11">
@@ -3018,31 +3042,31 @@
         <v>28</v>
       </c>
       <c r="B11" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="D11" t="n">
-        <v>0.859122269183519</v>
+        <v>0.836837385227116</v>
       </c>
       <c r="E11" t="n">
-        <v>0.78080961686178</v>
+        <v>0.81554061575129</v>
       </c>
       <c r="F11" t="n">
-        <v>0.918746792678755</v>
+        <v>0.865310704022988</v>
       </c>
       <c r="G11" t="n">
-        <v>0.897810218978102</v>
+        <v>0.871046228710462</v>
       </c>
       <c r="H11" t="n">
-        <v>0.800066775986594</v>
+        <v>0.714796648667585</v>
       </c>
       <c r="I11" t="n">
-        <v>0.743114131000729</v>
+        <v>0.611798780487805</v>
       </c>
       <c r="J11" t="n">
-        <v>0.851420454545455</v>
+        <v>0.784967320261438</v>
       </c>
     </row>
     <row r="12">
@@ -3050,31 +3074,31 @@
         <v>30</v>
       </c>
       <c r="B12" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="D12" t="n">
-        <v>0.56678360807247</v>
+        <v>0.70541693445539</v>
       </c>
       <c r="E12" t="n">
-        <v>0.49450968181347</v>
+        <v>0.676296906310832</v>
       </c>
       <c r="F12" t="n">
-        <v>0.644056316046245</v>
+        <v>0.732316940322575</v>
       </c>
       <c r="G12" t="n">
-        <v>0.770773638968481</v>
+        <v>0.796666666666667</v>
       </c>
       <c r="H12" t="n">
-        <v>0.563603554158525</v>
+        <v>0.666520990079611</v>
       </c>
       <c r="I12" t="n">
-        <v>0.496016260162602</v>
+        <v>0.630497400266875</v>
       </c>
       <c r="J12" t="n">
-        <v>0.622742946708464</v>
+        <v>0.715919750408066</v>
       </c>
     </row>
     <row r="13">
@@ -3082,31 +3106,31 @@
         <v>32</v>
       </c>
       <c r="B13" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D13" t="n">
-        <v>0.876440598758502</v>
+        <v>0.815841149991267</v>
       </c>
       <c r="E13" t="n">
-        <v>0.810955578512397</v>
+        <v>0.767245697493333</v>
       </c>
       <c r="F13" t="n">
-        <v>0.957397959183673</v>
+        <v>0.867606281947807</v>
       </c>
       <c r="G13" t="n">
-        <v>0.893719806763285</v>
+        <v>0.868884540117417</v>
       </c>
       <c r="H13" t="n">
-        <v>0.774346650316729</v>
+        <v>0.751584108985944</v>
       </c>
       <c r="I13" t="n">
-        <v>0.691049190535492</v>
+        <v>0.703027352594874</v>
       </c>
       <c r="J13" t="n">
-        <v>0.82401988908013</v>
+        <v>0.805905989824237</v>
       </c>
     </row>
   </sheetData>
@@ -3394,7 +3418,7 @@
         <v>22</v>
       </c>
       <c r="B8" t="n">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
         <v>37</v>
@@ -3406,25 +3430,25 @@
         <v>38</v>
       </c>
       <c r="F8" t="n">
-        <v>0.979444043637531</v>
+        <v>0.985350227678353</v>
       </c>
       <c r="G8" t="n">
-        <v>0.934172491970527</v>
+        <v>0.960316059306447</v>
       </c>
       <c r="H8" t="n">
-        <v>0.999863387978142</v>
+        <v>0.997564793250785</v>
       </c>
       <c r="I8" t="n">
         <v>1</v>
       </c>
       <c r="J8" t="n">
-        <v>0.946336161818759</v>
+        <v>0.935729391768742</v>
       </c>
       <c r="K8" t="n">
-        <v>0.911337464356218</v>
+        <v>0.896362229102167</v>
       </c>
       <c r="L8" t="n">
-        <v>0.977858056265985</v>
+        <v>0.971176470588235</v>
       </c>
     </row>
     <row r="9">
@@ -3432,37 +3456,37 @@
         <v>24</v>
       </c>
       <c r="B9" t="n">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
         <v>37</v>
       </c>
       <c r="D9" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E9" t="s">
         <v>38</v>
       </c>
       <c r="F9" t="n">
-        <v>0.716214690163669</v>
+        <v>0.847381516200544</v>
       </c>
       <c r="G9" t="n">
-        <v>0.586080102338356</v>
+        <v>0.797293003512881</v>
       </c>
       <c r="H9" t="n">
-        <v>0.805050429504952</v>
+        <v>0.881652437489837</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0.620539609809178</v>
+        <v>0.74776497733605</v>
       </c>
       <c r="K9" t="n">
-        <v>0.550829462508295</v>
+        <v>0.710100826596421</v>
       </c>
       <c r="L9" t="n">
-        <v>0.701793785310734</v>
+        <v>0.799396396396396</v>
       </c>
     </row>
     <row r="10">
@@ -3470,37 +3494,37 @@
         <v>26</v>
       </c>
       <c r="B10" t="n">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
         <v>37</v>
       </c>
       <c r="D10" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E10" t="s">
         <v>38</v>
       </c>
       <c r="F10" t="n">
-        <v>0.927119091597584</v>
+        <v>0.95606497902966</v>
       </c>
       <c r="G10" t="n">
-        <v>0.776994916003537</v>
+        <v>0.932736938548771</v>
       </c>
       <c r="H10" t="n">
-        <v>0.997339650145773</v>
+        <v>0.976707732329954</v>
       </c>
       <c r="I10" t="n">
         <v>1</v>
       </c>
       <c r="J10" t="n">
-        <v>0.878714601389206</v>
+        <v>0.900810945507319</v>
       </c>
       <c r="K10" t="n">
-        <v>0.647757090488134</v>
+        <v>0.883334860703812</v>
       </c>
       <c r="L10" t="n">
-        <v>0.967264295276343</v>
+        <v>0.911624747219414</v>
       </c>
     </row>
     <row r="11">
@@ -3508,37 +3532,37 @@
         <v>28</v>
       </c>
       <c r="B11" t="n">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
         <v>37</v>
       </c>
       <c r="D11" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E11" t="s">
         <v>38</v>
       </c>
       <c r="F11" t="n">
-        <v>0.929454441984135</v>
+        <v>0.966646749769644</v>
       </c>
       <c r="G11" t="n">
-        <v>0.812141112379545</v>
+        <v>0.947824341811731</v>
       </c>
       <c r="H11" t="n">
-        <v>0.986969151528578</v>
+        <v>0.99151550065781</v>
       </c>
       <c r="I11" t="n">
         <v>1</v>
       </c>
       <c r="J11" t="n">
-        <v>0.867413476271387</v>
+        <v>0.905013611923847</v>
       </c>
       <c r="K11" t="n">
-        <v>0.769463249516441</v>
+        <v>0.861336190105181</v>
       </c>
       <c r="L11" t="n">
-        <v>0.920156320035858</v>
+        <v>0.949637096774194</v>
       </c>
     </row>
     <row r="12">
@@ -3546,7 +3570,7 @@
         <v>30</v>
       </c>
       <c r="B12" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
         <v>37</v>
@@ -3558,25 +3582,25 @@
         <v>38</v>
       </c>
       <c r="F12" t="n">
-        <v>0.671099748143296</v>
+        <v>0.820050377501411</v>
       </c>
       <c r="G12" t="n">
-        <v>0.600333634328499</v>
+        <v>0.770538939650966</v>
       </c>
       <c r="H12" t="n">
-        <v>0.726968355478831</v>
+        <v>0.873856476282963</v>
       </c>
       <c r="I12" t="n">
         <v>1</v>
       </c>
       <c r="J12" t="n">
-        <v>0.629791341027629</v>
+        <v>0.725394234081725</v>
       </c>
       <c r="K12" t="n">
-        <v>0.585246598639456</v>
+        <v>0.687680025767266</v>
       </c>
       <c r="L12" t="n">
-        <v>0.69185791166646</v>
+        <v>0.777597471022129</v>
       </c>
     </row>
     <row r="13">
@@ -3584,37 +3608,37 @@
         <v>32</v>
       </c>
       <c r="B13" t="n">
-        <v>79</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
         <v>37</v>
       </c>
       <c r="D13" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E13" t="s">
         <v>38</v>
       </c>
       <c r="F13" t="n">
-        <v>0.948964657355045</v>
+        <v>0.944232362436968</v>
       </c>
       <c r="G13" t="n">
-        <v>0.905653320034198</v>
+        <v>0.898683535108959</v>
       </c>
       <c r="H13" t="n">
-        <v>0.999489795918367</v>
+        <v>0.982449992507788</v>
       </c>
       <c r="I13" t="n">
         <v>1</v>
       </c>
       <c r="J13" t="n">
-        <v>0.920141987157532</v>
+        <v>0.89221635822937</v>
       </c>
       <c r="K13" t="n">
-        <v>0.84583866837388</v>
+        <v>0.850862674154876</v>
       </c>
       <c r="L13" t="n">
-        <v>0.994303797468354</v>
+        <v>0.922178593086719</v>
       </c>
     </row>
   </sheetData>
@@ -3926,7 +3950,7 @@
         <v>500</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D8" t="n">
         <v>0.1</v>
@@ -3938,25 +3962,25 @@
         <v>38</v>
       </c>
       <c r="G8" t="n">
-        <v>0.970244457447449</v>
+        <v>0.982054545407962</v>
       </c>
       <c r="H8" t="n">
-        <v>0.922612318388726</v>
+        <v>0.969081199699177</v>
       </c>
       <c r="I8" t="n">
-        <v>0.997127303479763</v>
+        <v>0.993824280564692</v>
       </c>
       <c r="J8" t="n">
         <v>1</v>
       </c>
       <c r="K8" t="n">
-        <v>0.937733462742529</v>
+        <v>0.929725582249967</v>
       </c>
       <c r="L8" t="n">
-        <v>0.871902535998281</v>
+        <v>0.888959311096212</v>
       </c>
       <c r="M8" t="n">
-        <v>0.977525252525252</v>
+        <v>0.963986013986014</v>
       </c>
     </row>
     <row r="9">
@@ -3973,31 +3997,31 @@
         <v>0.1</v>
       </c>
       <c r="E9" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F9" t="s">
         <v>38</v>
       </c>
       <c r="G9" t="n">
-        <v>0.753122467293587</v>
+        <v>0.830245400589896</v>
       </c>
       <c r="H9" t="n">
-        <v>0.671409294086224</v>
+        <v>0.776004579971524</v>
       </c>
       <c r="I9" t="n">
-        <v>0.818063642453823</v>
+        <v>0.868754778152731</v>
       </c>
       <c r="J9" t="n">
         <v>1</v>
       </c>
       <c r="K9" t="n">
-        <v>0.688634850809322</v>
+        <v>0.752369965040683</v>
       </c>
       <c r="L9" t="n">
-        <v>0.606508684405026</v>
+        <v>0.702477064220183</v>
       </c>
       <c r="M9" t="n">
-        <v>0.752120105201636</v>
+        <v>0.801991347783427</v>
       </c>
     </row>
     <row r="10">
@@ -4008,37 +4032,37 @@
         <v>500</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D10" t="n">
         <v>0.1</v>
       </c>
       <c r="E10" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F10" t="s">
         <v>38</v>
       </c>
       <c r="G10" t="n">
-        <v>0.948864187334331</v>
+        <v>0.976455269222007</v>
       </c>
       <c r="H10" t="n">
-        <v>0.899053460906909</v>
+        <v>0.956809968666702</v>
       </c>
       <c r="I10" t="n">
-        <v>0.998809523809524</v>
+        <v>0.987460555578764</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>
       </c>
       <c r="K10" t="n">
-        <v>0.910749687059745</v>
+        <v>0.927314083514312</v>
       </c>
       <c r="L10" t="n">
-        <v>0.854698051321628</v>
+        <v>0.898330832708177</v>
       </c>
       <c r="M10" t="n">
-        <v>0.994578313253012</v>
+        <v>0.950966017677974</v>
       </c>
     </row>
     <row r="11">
@@ -4046,40 +4070,40 @@
         <v>28</v>
       </c>
       <c r="B11" t="n">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="C11" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D11" t="n">
         <v>0.1</v>
       </c>
       <c r="E11" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F11" t="s">
         <v>38</v>
       </c>
       <c r="G11" t="n">
-        <v>0.97448337478107</v>
+        <v>0.9710846568851</v>
       </c>
       <c r="H11" t="n">
-        <v>0.950006631299735</v>
+        <v>0.950317243085425</v>
       </c>
       <c r="I11" t="n">
-        <v>0.991735776277724</v>
+        <v>0.985565977570273</v>
       </c>
       <c r="J11" t="n">
         <v>1</v>
       </c>
       <c r="K11" t="n">
-        <v>0.924535703584486</v>
+        <v>0.906435007997149</v>
       </c>
       <c r="L11" t="n">
-        <v>0.881060606060606</v>
+        <v>0.869225993377484</v>
       </c>
       <c r="M11" t="n">
-        <v>0.965449910354101</v>
+        <v>0.92735294117647</v>
       </c>
     </row>
     <row r="12">
@@ -4090,7 +4114,7 @@
         <v>500</v>
       </c>
       <c r="C12" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D12" t="n">
         <v>0.1</v>
@@ -4102,25 +4126,25 @@
         <v>38</v>
       </c>
       <c r="G12" t="n">
-        <v>0.723648900971963</v>
+        <v>0.826982584599064</v>
       </c>
       <c r="H12" t="n">
-        <v>0.614136053685234</v>
+        <v>0.782315000410745</v>
       </c>
       <c r="I12" t="n">
-        <v>0.775485573173028</v>
+        <v>0.881889572330974</v>
       </c>
       <c r="J12" t="n">
         <v>1</v>
       </c>
       <c r="K12" t="n">
-        <v>0.675719323413781</v>
+        <v>0.741893386105981</v>
       </c>
       <c r="L12" t="n">
-        <v>0.587575114881584</v>
+        <v>0.694778651443343</v>
       </c>
       <c r="M12" t="n">
-        <v>0.710032166752445</v>
+        <v>0.791978021978022</v>
       </c>
     </row>
     <row r="13">
@@ -4131,37 +4155,37 @@
         <v>500</v>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D13" t="n">
         <v>0.1</v>
       </c>
       <c r="E13" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F13" t="s">
         <v>38</v>
       </c>
       <c r="G13" t="n">
-        <v>0.966928449998739</v>
+        <v>0.968063247723867</v>
       </c>
       <c r="H13" t="n">
-        <v>0.913697474570985</v>
+        <v>0.94257104007104</v>
       </c>
       <c r="I13" t="n">
-        <v>0.995280612244898</v>
+        <v>0.988610813248911</v>
       </c>
       <c r="J13" t="n">
         <v>1</v>
       </c>
       <c r="K13" t="n">
-        <v>0.935080493503977</v>
+        <v>0.920555543859912</v>
       </c>
       <c r="L13" t="n">
-        <v>0.823675635904982</v>
+        <v>0.883039475105303</v>
       </c>
       <c r="M13" t="n">
-        <v>0.975629098673174</v>
+        <v>0.953096275940491</v>
       </c>
     </row>
   </sheetData>

</xml_diff>